<commit_message>
Created a new centralized xls file for all funds.
</commit_message>
<xml_diff>
--- a/FonduriInvestitii/data/INGDXCH.xlsx
+++ b/FonduriInvestitii/data/INGDXCH.xlsx
@@ -9,14 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INGDXCH" sheetId="1" r:id="rId1"/>
-    <sheet name="Graphs" sheetId="2" r:id="rId2"/>
+    <sheet name="INGROME" sheetId="3" r:id="rId2"/>
+    <sheet name="Graphs" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="INGROME_1" localSheetId="1">INGROME!$A$1:$B$257</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,8 +28,21 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="INGROME" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="D:\work\test_python\financial\FonduriInvestitii\main\INGROME.csv" tab="0" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -37,13 +53,19 @@
     <t>1-day</t>
   </si>
   <si>
-    <t>transaction</t>
-  </si>
-  <si>
     <t>max. randament[%]</t>
   </si>
   <si>
     <t>act. Randament[%]</t>
+  </si>
+  <si>
+    <t>pos.gain</t>
+  </si>
+  <si>
+    <t>elliot-analysis</t>
+  </si>
+  <si>
+    <t>open-pos1</t>
   </si>
 </sst>
 </file>
@@ -80,10 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -211,10 +234,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.9833307123761599E-2"/>
+          <c:x val="9.830662429057456E-2"/>
           <c:y val="3.9274376417233602E-2"/>
-          <c:w val="0.83008334643811899"/>
-          <c:h val="0.86566893424036295"/>
+          <c:w val="0.82160999603021989"/>
+          <c:h val="0.7334695046291877"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -263,10 +286,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>INGDXCH!$A$100:$A$178</c:f>
+              <c:f>INGDXCH!$A$100:$A$180</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd</c:formatCode>
-                <c:ptCount val="79"/>
+                <c:ptCount val="81"/>
                 <c:pt idx="0">
                   <c:v>42815</c:v>
                 </c:pt>
@@ -503,16 +526,22 @@
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>42933</c:v>
+                </c:pt>
+                <c:pt idx="79" formatCode="m/d/yyyy">
+                  <c:v>42934</c:v>
+                </c:pt>
+                <c:pt idx="80" formatCode="m/d/yyyy">
+                  <c:v>42935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>INGDXCH!$B$100:$B$178</c:f>
+              <c:f>INGDXCH!$B$100:$B$180</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="79"/>
+                <c:ptCount val="81"/>
                 <c:pt idx="0">
                   <c:v>1055.45</c:v>
                 </c:pt>
@@ -749,6 +778,12 @@
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>1069.68</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1065.6400000000001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1070.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -772,11 +807,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-177279552"/>
-        <c:axId val="-177279008"/>
+        <c:axId val="-984673584"/>
+        <c:axId val="-988260880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-177279552"/>
+        <c:axId val="-984673584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,14 +848,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-177279008"/>
+        <c:crossAx val="-988260880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-177279008"/>
+        <c:axId val="-988260880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +901,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-177279552"/>
+        <c:crossAx val="-984673584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -879,27 +914,6 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
@@ -924,16 +938,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>414360</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>630000</xdr:colOff>
-      <xdr:row>177</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -953,6 +967,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="INGROME_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1218,21 +1236,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D181"/>
+  <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.42578125"/>
-    <col min="2" max="2" width="8"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="18.42578125"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col min="4" max="4" width="11.5703125"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1243,10 +1263,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42676</v>
       </c>
@@ -1254,7 +1277,7 @@
         <v>991.83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42677</v>
       </c>
@@ -1266,7 +1289,7 @@
         <v>-0.14821088291340526</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42678</v>
       </c>
@@ -1278,7 +1301,7 @@
         <v>-0.3069590855850361</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42681</v>
       </c>
@@ -1290,7 +1313,7 @@
         <v>1.0786776323785578</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42682</v>
       </c>
@@ -1302,7 +1325,7 @@
         <v>-3.0061023878480135E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>42683</v>
       </c>
@@ -1314,7 +1337,7 @@
         <v>0.60741527759680647</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>42684</v>
       </c>
@@ -1326,7 +1349,7 @@
         <v>0.24110069440984716</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>42685</v>
       </c>
@@ -1338,7 +1361,7 @@
         <v>-0.27033742483725365</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>42688</v>
       </c>
@@ -1350,7 +1373,7 @@
         <v>0.4135814157440072</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>42689</v>
       </c>
@@ -1362,7 +1385,7 @@
         <v>0.13199944421285925</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>42690</v>
       </c>
@@ -1374,7 +1397,7 @@
         <v>5.1540771723937895E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>42691</v>
       </c>
@@ -1386,7 +1409,7 @@
         <v>0.15850529506751562</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>42692</v>
       </c>
@@ -1398,7 +1421,7 @@
         <v>5.242178768186629E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>42695</v>
       </c>
@@ -1410,7 +1433,7 @@
         <v>0.13049151805133161</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>42696</v>
       </c>
@@ -3150,7 +3173,7 @@
         <v>-0.24490704664366952</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>42914</v>
       </c>
@@ -3162,7 +3185,7 @@
         <v>-0.11531451102927585</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>42915</v>
       </c>
@@ -3174,7 +3197,7 @@
         <v>3.7241173841765624E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>42916</v>
       </c>
@@ -3182,11 +3205,11 @@
         <v>1074.74</v>
       </c>
       <c r="C163">
-        <f t="shared" ref="C163:C178" si="5">(B163-B162)*100/B162</f>
+        <f t="shared" ref="C163:C180" si="5">(B163-B162)*100/B162</f>
         <v>5.7721669832059577E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>42917</v>
       </c>
@@ -3198,7 +3221,7 @@
         <v>-0.45871559633028114</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>42918</v>
       </c>
@@ -3210,7 +3233,7 @@
         <v>-0.24770753685232552</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>42919</v>
       </c>
@@ -3222,7 +3245,7 @@
         <v>-1.0401439334308009</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>42920</v>
       </c>
@@ -3234,7 +3257,7 @@
         <v>1.1362990739173745E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>42921</v>
       </c>
@@ -3246,7 +3269,7 @@
         <v>0.20261697816658833</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>42922</v>
       </c>
@@ -3258,7 +3281,7 @@
         <v>5.9528309018076687E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>42923</v>
       </c>
@@ -3270,7 +3293,7 @@
         <v>0.28141083148401891</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>42924</v>
       </c>
@@ -3281,8 +3304,12 @@
         <f t="shared" si="5"/>
         <v>-0.68177751829216693</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E171">
+        <f>B171/B171</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>42925</v>
       </c>
@@ -3293,8 +3320,12 @@
         <f t="shared" si="5"/>
         <v>0.16497738672026938</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E172">
+        <f>B172-B171</f>
+        <v>1.7400000000000091</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>42926</v>
       </c>
@@ -3305,8 +3336,12 @@
         <f t="shared" si="5"/>
         <v>0.21866096191891041</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E173">
+        <f>B173-B171</f>
+        <v>4.0499999999999545</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>42927</v>
       </c>
@@ -3317,8 +3352,12 @@
         <f t="shared" si="5"/>
         <v>-9.3507376693051092E-2</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E174">
+        <f>B174-B171</f>
+        <v>3.0599999999999454</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>42928</v>
       </c>
@@ -3329,8 +3368,12 @@
         <f t="shared" si="5"/>
         <v>0.65138265185536282</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E175">
+        <f>B175-B171</f>
+        <v>9.9500000000000455</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>42929</v>
       </c>
@@ -3344,8 +3387,12 @@
       <c r="D176">
         <v>2000</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E176">
+        <f>B176-B171</f>
+        <v>12.669999999999845</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>42930</v>
       </c>
@@ -3356,8 +3403,16 @@
         <f t="shared" si="5"/>
         <v>0.11804826862539265</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D177">
+        <f>B177/B176*D176</f>
+        <v>2002.360965372508</v>
+      </c>
+      <c r="E177">
+        <f>B177-B171</f>
+        <v>13.929999999999836</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>42933</v>
       </c>
@@ -3368,23 +3423,91 @@
         <f t="shared" si="5"/>
         <v>9.9193352173847851E-2</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C180" t="s">
+      <c r="D178">
+        <f t="shared" ref="D178:D180" si="6">B178/B177*D177</f>
+        <v>2004.3471743366817</v>
+      </c>
+      <c r="E178">
+        <f>B178-B171</f>
+        <v>14.990000000000009</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
+        <v>42934</v>
+      </c>
+      <c r="B179">
+        <v>1065.6400000000001</v>
+      </c>
+      <c r="C179">
+        <f t="shared" si="5"/>
+        <v>-0.37768304539675074</v>
+      </c>
+      <c r="D179">
+        <f t="shared" si="6"/>
+        <v>1996.7770948883233</v>
+      </c>
+      <c r="E179">
+        <f>B179-B171</f>
+        <v>10.950000000000045</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" s="3">
+        <v>42935</v>
+      </c>
+      <c r="B180">
+        <v>1070.54</v>
+      </c>
+      <c r="C180">
+        <f t="shared" si="5"/>
+        <v>0.45981757441536197</v>
+      </c>
+      <c r="D180">
+        <f t="shared" si="6"/>
+        <v>2005.9586268925202</v>
+      </c>
+      <c r="E180">
+        <f>B180-B171</f>
+        <v>15.849999999999909</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" s="3"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="3"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C183" t="s">
+        <v>5</v>
+      </c>
+      <c r="D183" s="2">
+        <f>D180-D176</f>
+        <v>5.9586268925202148</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B184" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184" s="2">
+        <f>SUMIF(C2:C180,"&gt;0",C2:C180)</f>
+        <v>25.40332861032606</v>
+      </c>
+      <c r="D184" s="2"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B185" t="s">
         <v>4</v>
       </c>
-      <c r="D180" s="2">
-        <f>SUMIF(C2:C178,"&gt;0",C2:C178)</f>
-        <v>24.943511035910699</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C181" t="s">
-        <v>5</v>
-      </c>
-      <c r="D181">
-        <f>(B178-B2)*100/B2</f>
-        <v>7.8491273706179499</v>
+      <c r="C185">
+        <f>(B180-B2)*100/B2</f>
+        <v>7.9358357783087747</v>
+      </c>
+      <c r="D185" s="2">
+        <f>(D180-D176)/D176*100</f>
+        <v>0.29793134462601073</v>
       </c>
     </row>
   </sheetData>
@@ -3399,6 +3522,2079 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B257"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>42566</v>
+      </c>
+      <c r="B2">
+        <v>903.92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>42569</v>
+      </c>
+      <c r="B3">
+        <v>909.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>42570</v>
+      </c>
+      <c r="B4">
+        <v>913.81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>42571</v>
+      </c>
+      <c r="B5">
+        <v>918.83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>42572</v>
+      </c>
+      <c r="B6">
+        <v>918.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>42573</v>
+      </c>
+      <c r="B7">
+        <v>918.29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>42576</v>
+      </c>
+      <c r="B8">
+        <v>921.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>42577</v>
+      </c>
+      <c r="B9">
+        <v>921.38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>42578</v>
+      </c>
+      <c r="B10">
+        <v>923.79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>42579</v>
+      </c>
+      <c r="B11">
+        <v>921.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>42580</v>
+      </c>
+      <c r="B12">
+        <v>921.67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>42583</v>
+      </c>
+      <c r="B13">
+        <v>920.84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>42584</v>
+      </c>
+      <c r="B14">
+        <v>918.92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>42585</v>
+      </c>
+      <c r="B15">
+        <v>913.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>42586</v>
+      </c>
+      <c r="B16">
+        <v>921.49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>42587</v>
+      </c>
+      <c r="B17">
+        <v>926.34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>42590</v>
+      </c>
+      <c r="B18">
+        <v>935.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>42591</v>
+      </c>
+      <c r="B19">
+        <v>940.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>42592</v>
+      </c>
+      <c r="B20">
+        <v>938.87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>42593</v>
+      </c>
+      <c r="B21">
+        <v>942.37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>42594</v>
+      </c>
+      <c r="B22">
+        <v>939.34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>42598</v>
+      </c>
+      <c r="B23">
+        <v>940.64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>42599</v>
+      </c>
+      <c r="B24">
+        <v>938.78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>42600</v>
+      </c>
+      <c r="B25">
+        <v>941.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>42601</v>
+      </c>
+      <c r="B26">
+        <v>938.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>42604</v>
+      </c>
+      <c r="B27">
+        <v>936.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>42605</v>
+      </c>
+      <c r="B28">
+        <v>938.56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>42606</v>
+      </c>
+      <c r="B29">
+        <v>945.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>42607</v>
+      </c>
+      <c r="B30">
+        <v>945.21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>42608</v>
+      </c>
+      <c r="B31">
+        <v>948.84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>42611</v>
+      </c>
+      <c r="B32">
+        <v>948.38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>42612</v>
+      </c>
+      <c r="B33">
+        <v>953.28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>42613</v>
+      </c>
+      <c r="B34">
+        <v>953.96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>42614</v>
+      </c>
+      <c r="B35">
+        <v>952.46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>42615</v>
+      </c>
+      <c r="B36">
+        <v>952.93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>42618</v>
+      </c>
+      <c r="B37">
+        <v>956.45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>42619</v>
+      </c>
+      <c r="B38">
+        <v>959.32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>42620</v>
+      </c>
+      <c r="B39">
+        <v>965.95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>42621</v>
+      </c>
+      <c r="B40">
+        <v>965.92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>42622</v>
+      </c>
+      <c r="B41">
+        <v>958.73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>42625</v>
+      </c>
+      <c r="B42">
+        <v>945.54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>42626</v>
+      </c>
+      <c r="B43">
+        <v>946.76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>42627</v>
+      </c>
+      <c r="B44">
+        <v>947.85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>42628</v>
+      </c>
+      <c r="B45">
+        <v>950.64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>42629</v>
+      </c>
+      <c r="B46">
+        <v>950.24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>42632</v>
+      </c>
+      <c r="B47">
+        <v>955.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>42633</v>
+      </c>
+      <c r="B48">
+        <v>953.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>42634</v>
+      </c>
+      <c r="B49">
+        <v>956.91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>42635</v>
+      </c>
+      <c r="B50">
+        <v>962.65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>42636</v>
+      </c>
+      <c r="B51">
+        <v>958.58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>42639</v>
+      </c>
+      <c r="B52">
+        <v>951.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>42640</v>
+      </c>
+      <c r="B53">
+        <v>947.67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>42641</v>
+      </c>
+      <c r="B54">
+        <v>948.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>42642</v>
+      </c>
+      <c r="B55">
+        <v>954.69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>42643</v>
+      </c>
+      <c r="B56">
+        <v>946.46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>42646</v>
+      </c>
+      <c r="B57">
+        <v>951.16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>42647</v>
+      </c>
+      <c r="B58">
+        <v>959.17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>42648</v>
+      </c>
+      <c r="B59">
+        <v>961.37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>42649</v>
+      </c>
+      <c r="B60">
+        <v>962.51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>42650</v>
+      </c>
+      <c r="B61">
+        <v>964.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>42653</v>
+      </c>
+      <c r="B62">
+        <v>962.85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>42654</v>
+      </c>
+      <c r="B63">
+        <v>961.41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>42655</v>
+      </c>
+      <c r="B64">
+        <v>960.83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>42656</v>
+      </c>
+      <c r="B65">
+        <v>954.64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
+        <v>42657</v>
+      </c>
+      <c r="B66">
+        <v>959.48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>42660</v>
+      </c>
+      <c r="B67">
+        <v>958.96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>42661</v>
+      </c>
+      <c r="B68">
+        <v>964.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>42662</v>
+      </c>
+      <c r="B69">
+        <v>970.25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>42663</v>
+      </c>
+      <c r="B70">
+        <v>972.32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
+        <v>42664</v>
+      </c>
+      <c r="B71">
+        <v>969.47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
+        <v>42667</v>
+      </c>
+      <c r="B72">
+        <v>972.91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
+        <v>42668</v>
+      </c>
+      <c r="B73">
+        <v>966.04</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>42669</v>
+      </c>
+      <c r="B74">
+        <v>966.62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>42670</v>
+      </c>
+      <c r="B75">
+        <v>969.94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>42671</v>
+      </c>
+      <c r="B76">
+        <v>972.3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
+        <v>42674</v>
+      </c>
+      <c r="B77">
+        <v>970.81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="3">
+        <v>42675</v>
+      </c>
+      <c r="B78">
+        <v>971.31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="3">
+        <v>42676</v>
+      </c>
+      <c r="B79">
+        <v>959.48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
+        <v>42677</v>
+      </c>
+      <c r="B80">
+        <v>963.76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3">
+        <v>42678</v>
+      </c>
+      <c r="B81">
+        <v>958.44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3">
+        <v>42681</v>
+      </c>
+      <c r="B82">
+        <v>962.74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3">
+        <v>42682</v>
+      </c>
+      <c r="B83">
+        <v>964.07</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="3">
+        <v>42683</v>
+      </c>
+      <c r="B84">
+        <v>960.44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="3">
+        <v>42684</v>
+      </c>
+      <c r="B85">
+        <v>965.42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="3">
+        <v>42685</v>
+      </c>
+      <c r="B86">
+        <v>965.39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="3">
+        <v>42688</v>
+      </c>
+      <c r="B87">
+        <v>961.83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="3">
+        <v>42689</v>
+      </c>
+      <c r="B88">
+        <v>963.38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="3">
+        <v>42690</v>
+      </c>
+      <c r="B89">
+        <v>959.73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="3">
+        <v>42691</v>
+      </c>
+      <c r="B90">
+        <v>959.28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="3">
+        <v>42692</v>
+      </c>
+      <c r="B91">
+        <v>954.93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="3">
+        <v>42695</v>
+      </c>
+      <c r="B92">
+        <v>958.1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="3">
+        <v>42696</v>
+      </c>
+      <c r="B93">
+        <v>962.15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="3">
+        <v>42697</v>
+      </c>
+      <c r="B94">
+        <v>961.66</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="3">
+        <v>42698</v>
+      </c>
+      <c r="B95">
+        <v>961.94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="3">
+        <v>42699</v>
+      </c>
+      <c r="B96">
+        <v>962.44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="3">
+        <v>42702</v>
+      </c>
+      <c r="B97">
+        <v>956.4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="3">
+        <v>42703</v>
+      </c>
+      <c r="B98">
+        <v>958.36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="3">
+        <v>42704</v>
+      </c>
+      <c r="B99">
+        <v>958.1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="3">
+        <v>42706</v>
+      </c>
+      <c r="B100">
+        <v>965.45</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="3">
+        <v>42709</v>
+      </c>
+      <c r="B101">
+        <v>966.47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="3">
+        <v>42710</v>
+      </c>
+      <c r="B102">
+        <v>966.41</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="3">
+        <v>42711</v>
+      </c>
+      <c r="B103">
+        <v>966.66</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="3">
+        <v>42712</v>
+      </c>
+      <c r="B104">
+        <v>969.45</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="3">
+        <v>42713</v>
+      </c>
+      <c r="B105">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="3">
+        <v>42716</v>
+      </c>
+      <c r="B106">
+        <v>973.17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
+        <v>42717</v>
+      </c>
+      <c r="B107">
+        <v>981.84</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
+        <v>42718</v>
+      </c>
+      <c r="B108">
+        <v>986.26</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>42719</v>
+      </c>
+      <c r="B109">
+        <v>985.58</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>42720</v>
+      </c>
+      <c r="B110">
+        <v>993.02</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>42723</v>
+      </c>
+      <c r="B111">
+        <v>993.86</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>42724</v>
+      </c>
+      <c r="B112">
+        <v>993.49</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>42725</v>
+      </c>
+      <c r="B113">
+        <v>993.25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>42726</v>
+      </c>
+      <c r="B114">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>42727</v>
+      </c>
+      <c r="B115">
+        <v>994.72</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>42731</v>
+      </c>
+      <c r="B116">
+        <v>997.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>42732</v>
+      </c>
+      <c r="B117">
+        <v>998.15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>42733</v>
+      </c>
+      <c r="B118">
+        <v>1001.42</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
+        <v>42734</v>
+      </c>
+      <c r="B119">
+        <v>1004.7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="3">
+        <v>42738</v>
+      </c>
+      <c r="B120">
+        <v>1015.17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>42739</v>
+      </c>
+      <c r="B121">
+        <v>1021.07</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>42740</v>
+      </c>
+      <c r="B122">
+        <v>1020.4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>42741</v>
+      </c>
+      <c r="B123">
+        <v>1022.9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>42744</v>
+      </c>
+      <c r="B124">
+        <v>1024.6500000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>42745</v>
+      </c>
+      <c r="B125">
+        <v>1024.8800000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
+        <v>42746</v>
+      </c>
+      <c r="B126">
+        <v>1025.6199999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="3">
+        <v>42747</v>
+      </c>
+      <c r="B127">
+        <v>1018.37</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
+        <v>42748</v>
+      </c>
+      <c r="B128">
+        <v>1015.81</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
+        <v>42751</v>
+      </c>
+      <c r="B129">
+        <v>1016.91</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
+        <v>42752</v>
+      </c>
+      <c r="B130">
+        <v>1015.74</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
+        <v>42753</v>
+      </c>
+      <c r="B131">
+        <v>1015.4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>42754</v>
+      </c>
+      <c r="B132">
+        <v>1019.66</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
+        <v>42755</v>
+      </c>
+      <c r="B133">
+        <v>1023.99</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="3">
+        <v>42758</v>
+      </c>
+      <c r="B134">
+        <v>1020.91</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>42759</v>
+      </c>
+      <c r="B135">
+        <v>1023.04</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>42760</v>
+      </c>
+      <c r="B136">
+        <v>1041.29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>42761</v>
+      </c>
+      <c r="B137">
+        <v>1042.43</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>42762</v>
+      </c>
+      <c r="B138">
+        <v>1051.8699999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="3">
+        <v>42765</v>
+      </c>
+      <c r="B139">
+        <v>1046.1199999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="3">
+        <v>42766</v>
+      </c>
+      <c r="B140">
+        <v>1050.1500000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="3">
+        <v>42767</v>
+      </c>
+      <c r="B141">
+        <v>1058.05</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="3">
+        <v>42768</v>
+      </c>
+      <c r="B142">
+        <v>1051.5999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
+        <v>42769</v>
+      </c>
+      <c r="B143">
+        <v>1054.8800000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
+        <v>42772</v>
+      </c>
+      <c r="B144">
+        <v>1062.76</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
+        <v>42773</v>
+      </c>
+      <c r="B145">
+        <v>1064.25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="3">
+        <v>42774</v>
+      </c>
+      <c r="B146">
+        <v>1063.2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="3">
+        <v>42775</v>
+      </c>
+      <c r="B147">
+        <v>1071.3900000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="3">
+        <v>42776</v>
+      </c>
+      <c r="B148">
+        <v>1080.68</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>42779</v>
+      </c>
+      <c r="B149">
+        <v>1080.71</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
+        <v>42780</v>
+      </c>
+      <c r="B150">
+        <v>1077.1400000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
+        <v>42781</v>
+      </c>
+      <c r="B151">
+        <v>1084.77</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
+        <v>42782</v>
+      </c>
+      <c r="B152">
+        <v>1090.1600000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
+        <v>42783</v>
+      </c>
+      <c r="B153">
+        <v>1089.45</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="3">
+        <v>42786</v>
+      </c>
+      <c r="B154">
+        <v>1095.55</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="3">
+        <v>42787</v>
+      </c>
+      <c r="B155">
+        <v>1110.6500000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
+        <v>42788</v>
+      </c>
+      <c r="B156">
+        <v>1119.8900000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
+        <v>42789</v>
+      </c>
+      <c r="B157">
+        <v>1118.43</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
+        <v>42790</v>
+      </c>
+      <c r="B158">
+        <v>1104.6099999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="3">
+        <v>42793</v>
+      </c>
+      <c r="B159">
+        <v>1106.53</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>42794</v>
+      </c>
+      <c r="B160">
+        <v>1100.47</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="3">
+        <v>42795</v>
+      </c>
+      <c r="B161">
+        <v>1117.21</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="3">
+        <v>42796</v>
+      </c>
+      <c r="B162">
+        <v>1110.6600000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="3">
+        <v>42797</v>
+      </c>
+      <c r="B163">
+        <v>1108.77</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="3">
+        <v>42800</v>
+      </c>
+      <c r="B164">
+        <v>1107.8900000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="3">
+        <v>42801</v>
+      </c>
+      <c r="B165">
+        <v>1103.0999999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="3">
+        <v>42802</v>
+      </c>
+      <c r="B166">
+        <v>1102.73</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="3">
+        <v>42803</v>
+      </c>
+      <c r="B167">
+        <v>1098.6600000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="3">
+        <v>42804</v>
+      </c>
+      <c r="B168">
+        <v>1100.5999999999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="3">
+        <v>42807</v>
+      </c>
+      <c r="B169">
+        <v>1105.51</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="3">
+        <v>42808</v>
+      </c>
+      <c r="B170">
+        <v>1105.1300000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="3">
+        <v>42809</v>
+      </c>
+      <c r="B171">
+        <v>1111.1600000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="3">
+        <v>42810</v>
+      </c>
+      <c r="B172">
+        <v>1118.6400000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="3">
+        <v>42811</v>
+      </c>
+      <c r="B173">
+        <v>1121.25</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="3">
+        <v>42814</v>
+      </c>
+      <c r="B174">
+        <v>1119.7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="3">
+        <v>42815</v>
+      </c>
+      <c r="B175">
+        <v>1116.6099999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="3">
+        <v>42816</v>
+      </c>
+      <c r="B176">
+        <v>1110.49</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="3">
+        <v>42817</v>
+      </c>
+      <c r="B177">
+        <v>1113.5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="3">
+        <v>42818</v>
+      </c>
+      <c r="B178">
+        <v>1114.33</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
+        <v>42821</v>
+      </c>
+      <c r="B179">
+        <v>1108.4100000000001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="3">
+        <v>42822</v>
+      </c>
+      <c r="B180">
+        <v>1113.22</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="3">
+        <v>42823</v>
+      </c>
+      <c r="B181">
+        <v>1111.1500000000001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="3">
+        <v>42824</v>
+      </c>
+      <c r="B182">
+        <v>1115.17</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="3">
+        <v>42825</v>
+      </c>
+      <c r="B183">
+        <v>1113.1600000000001</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="3">
+        <v>42828</v>
+      </c>
+      <c r="B184">
+        <v>1123.33</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="3">
+        <v>42829</v>
+      </c>
+      <c r="B185">
+        <v>1124.8499999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="3">
+        <v>42830</v>
+      </c>
+      <c r="B186">
+        <v>1129.8699999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="3">
+        <v>42831</v>
+      </c>
+      <c r="B187">
+        <v>1132.5899999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="3">
+        <v>42832</v>
+      </c>
+      <c r="B188">
+        <v>1135.1199999999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="3">
+        <v>42835</v>
+      </c>
+      <c r="B189">
+        <v>1133.45</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="3">
+        <v>42836</v>
+      </c>
+      <c r="B190">
+        <v>1127.55</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="3">
+        <v>42837</v>
+      </c>
+      <c r="B191">
+        <v>1127.68</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="3">
+        <v>42838</v>
+      </c>
+      <c r="B192">
+        <v>1132.6300000000001</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="3">
+        <v>42843</v>
+      </c>
+      <c r="B193">
+        <v>1130.77</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="3">
+        <v>42844</v>
+      </c>
+      <c r="B194">
+        <v>1131.8499999999999</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="3">
+        <v>42845</v>
+      </c>
+      <c r="B195">
+        <v>1134.23</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="3">
+        <v>42846</v>
+      </c>
+      <c r="B196">
+        <v>1133.8499999999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="3">
+        <v>42849</v>
+      </c>
+      <c r="B197">
+        <v>1145.51</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="3">
+        <v>42850</v>
+      </c>
+      <c r="B198">
+        <v>1150.9100000000001</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="3">
+        <v>42851</v>
+      </c>
+      <c r="B199">
+        <v>1153.94</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="3">
+        <v>42852</v>
+      </c>
+      <c r="B200">
+        <v>1148.71</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="3">
+        <v>42853</v>
+      </c>
+      <c r="B201">
+        <v>1154.07</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="3">
+        <v>42857</v>
+      </c>
+      <c r="B202">
+        <v>1156.94</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="3">
+        <v>42858</v>
+      </c>
+      <c r="B203">
+        <v>1154.5999999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="3">
+        <v>42859</v>
+      </c>
+      <c r="B204">
+        <v>1155.6199999999999</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="3">
+        <v>42860</v>
+      </c>
+      <c r="B205">
+        <v>1163.51</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="3">
+        <v>42863</v>
+      </c>
+      <c r="B206">
+        <v>1165.8599999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="3">
+        <v>42864</v>
+      </c>
+      <c r="B207">
+        <v>1174.73</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="3">
+        <v>42865</v>
+      </c>
+      <c r="B208">
+        <v>1173.68</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="3">
+        <v>42866</v>
+      </c>
+      <c r="B209">
+        <v>1177.3399999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="3">
+        <v>42867</v>
+      </c>
+      <c r="B210">
+        <v>1183.3699999999999</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="3">
+        <v>42870</v>
+      </c>
+      <c r="B211">
+        <v>1191.22</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="3">
+        <v>42871</v>
+      </c>
+      <c r="B212">
+        <v>1187.45</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="3">
+        <v>42872</v>
+      </c>
+      <c r="B213">
+        <v>1183.01</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="3">
+        <v>42873</v>
+      </c>
+      <c r="B214">
+        <v>1177.04</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="3">
+        <v>42874</v>
+      </c>
+      <c r="B215">
+        <v>1187.1199999999999</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="3">
+        <v>42877</v>
+      </c>
+      <c r="B216">
+        <v>1193.98</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="3">
+        <v>42878</v>
+      </c>
+      <c r="B217">
+        <v>1187.8800000000001</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="3">
+        <v>42879</v>
+      </c>
+      <c r="B218">
+        <v>1192.73</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="3">
+        <v>42880</v>
+      </c>
+      <c r="B219">
+        <v>1200.9100000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="3">
+        <v>42881</v>
+      </c>
+      <c r="B220">
+        <v>1202.74</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="3">
+        <v>42884</v>
+      </c>
+      <c r="B221">
+        <v>1204.2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="3">
+        <v>42885</v>
+      </c>
+      <c r="B222">
+        <v>1203.6300000000001</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="3">
+        <v>42886</v>
+      </c>
+      <c r="B223">
+        <v>1209.68</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="3">
+        <v>42887</v>
+      </c>
+      <c r="B224">
+        <v>1209.71</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="3">
+        <v>42888</v>
+      </c>
+      <c r="B225">
+        <v>1213.33</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="3">
+        <v>42892</v>
+      </c>
+      <c r="B226">
+        <v>1210.3399999999999</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="3">
+        <v>42893</v>
+      </c>
+      <c r="B227">
+        <v>1212.55</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="3">
+        <v>42894</v>
+      </c>
+      <c r="B228">
+        <v>1213.25</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="3">
+        <v>42895</v>
+      </c>
+      <c r="B229">
+        <v>1207.8800000000001</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="3">
+        <v>42898</v>
+      </c>
+      <c r="B230">
+        <v>1197.3499999999999</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="3">
+        <v>42899</v>
+      </c>
+      <c r="B231">
+        <v>1199.71</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="3">
+        <v>42900</v>
+      </c>
+      <c r="B232">
+        <v>1203.79</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="3">
+        <v>42901</v>
+      </c>
+      <c r="B233">
+        <v>1194.25</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="3">
+        <v>42902</v>
+      </c>
+      <c r="B234">
+        <v>1199.57</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="3">
+        <v>42905</v>
+      </c>
+      <c r="B235">
+        <v>1200.03</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="3">
+        <v>42906</v>
+      </c>
+      <c r="B236">
+        <v>1193.03</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="3">
+        <v>42907</v>
+      </c>
+      <c r="B237">
+        <v>1193.01</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="3">
+        <v>42908</v>
+      </c>
+      <c r="B238">
+        <v>1185.98</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="3">
+        <v>42909</v>
+      </c>
+      <c r="B239">
+        <v>1186.19</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="3">
+        <v>42912</v>
+      </c>
+      <c r="B240">
+        <v>1189.17</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="3">
+        <v>42913</v>
+      </c>
+      <c r="B241">
+        <v>1184.45</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="3">
+        <v>42914</v>
+      </c>
+      <c r="B242">
+        <v>1177.8699999999999</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="3">
+        <v>42915</v>
+      </c>
+      <c r="B243">
+        <v>1156.1099999999999</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="3">
+        <v>42916</v>
+      </c>
+      <c r="B244">
+        <v>1154.32</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="3">
+        <v>42919</v>
+      </c>
+      <c r="B245">
+        <v>1156.67</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="3">
+        <v>42920</v>
+      </c>
+      <c r="B246">
+        <v>1168.9000000000001</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="3">
+        <v>42921</v>
+      </c>
+      <c r="B247">
+        <v>1188.6199999999999</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="3">
+        <v>42922</v>
+      </c>
+      <c r="B248">
+        <v>1184.8399999999999</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="3">
+        <v>42923</v>
+      </c>
+      <c r="B249">
+        <v>1179.5899999999999</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="3">
+        <v>42926</v>
+      </c>
+      <c r="B250">
+        <v>1185.57</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" s="3">
+        <v>42927</v>
+      </c>
+      <c r="B251">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" s="3">
+        <v>42928</v>
+      </c>
+      <c r="B252">
+        <v>1195.58</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" s="3">
+        <v>42929</v>
+      </c>
+      <c r="B253">
+        <v>1198.56</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" s="3">
+        <v>42930</v>
+      </c>
+      <c r="B254">
+        <v>1197.74</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" s="3">
+        <v>42933</v>
+      </c>
+      <c r="B255">
+        <v>1202.97</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" s="3">
+        <v>42934</v>
+      </c>
+      <c r="B256">
+        <v>1207.58</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" s="3">
+        <v>42935</v>
+      </c>
+      <c r="B257">
+        <v>1212.52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>